<commit_message>
add Gariguette_2.mtg and Nils_2.mtg with label modification and PO indexation
</commit_message>
<xml_diff>
--- a/Index codification.xlsx
+++ b/Index codification.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="126">
   <si>
     <t>Label</t>
   </si>
@@ -165,9 +165,6 @@
     <t>PO:0000055</t>
   </si>
   <si>
-    <t>diameter of collar (of the Primary crown)</t>
-  </si>
-  <si>
     <t>Leaf area</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>Synonyms</t>
   </si>
   <si>
-    <t>leaflet width</t>
-  </si>
-  <si>
     <t>leaflet lenght (mm)</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>Leaf area (mm²)</t>
   </si>
   <si>
-    <t>leaflet length</t>
-  </si>
-  <si>
     <t>Left Leaflet area (mm²)</t>
   </si>
   <si>
@@ -382,6 +373,36 @@
   </si>
   <si>
     <t>Stage from I to 87 (Inflorescence stage)</t>
+  </si>
+  <si>
+    <t>Foliar type</t>
+  </si>
+  <si>
+    <t>Cotyledon, Unifoliate, Trifoliate, Trifoliate non developped, primordia foliar</t>
+  </si>
+  <si>
+    <t>Collar diameter (of the Primary crown)</t>
+  </si>
+  <si>
+    <t>Right leaflet length</t>
+  </si>
+  <si>
+    <t>Right leaflet width</t>
+  </si>
+  <si>
+    <t>Central leaflet width</t>
+  </si>
+  <si>
+    <t>Central leaflet length</t>
+  </si>
+  <si>
+    <t>Central  Leaflet area</t>
+  </si>
+  <si>
+    <t>Left leaflet width</t>
+  </si>
+  <si>
+    <t>Left leaflet length</t>
   </si>
 </sst>
 </file>
@@ -713,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A1:G37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,7 +746,7 @@
     <col min="2" max="2" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.44140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -747,7 +768,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G1" t="s">
         <v>21</v>
@@ -807,7 +828,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -821,16 +842,16 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -844,398 +865,398 @@
         <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" t="s">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" t="s">
-        <v>55</v>
-      </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="G13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>37</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="D14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D15" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
-      </c>
       <c r="G15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
         <v>57</v>
       </c>
-      <c r="F16" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D17" t="s">
+      <c r="G17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" t="s">
+        <v>105</v>
+      </c>
+      <c r="J22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>70</v>
+      </c>
+      <c r="E24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F24" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" t="s">
+        <v>108</v>
+      </c>
+      <c r="G25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" t="s">
+        <v>84</v>
+      </c>
+      <c r="E30" t="s">
         <v>85</v>
       </c>
-      <c r="E17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="F30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" t="s">
         <v>83</v>
       </c>
-      <c r="G17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" t="s">
-        <v>105</v>
-      </c>
-      <c r="G18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D19" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" t="s">
-        <v>106</v>
-      </c>
-      <c r="G19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" t="s">
-        <v>108</v>
-      </c>
-      <c r="G21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" t="s">
-        <v>65</v>
-      </c>
-      <c r="F22" t="s">
-        <v>109</v>
-      </c>
-      <c r="G22" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" t="s">
-        <v>110</v>
-      </c>
-      <c r="G23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" t="s">
-        <v>111</v>
-      </c>
-      <c r="G24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G25" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" t="s">
-        <v>113</v>
-      </c>
-      <c r="G26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D27" t="s">
-        <v>85</v>
-      </c>
-      <c r="E27" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" t="s">
         <v>87</v>
       </c>
-      <c r="E29" t="s">
-        <v>88</v>
-      </c>
-      <c r="F29" t="s">
-        <v>89</v>
-      </c>
-      <c r="G29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D30" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" t="s">
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" t="s">
         <v>94</v>
-      </c>
-      <c r="F30" t="s">
-        <v>92</v>
-      </c>
-      <c r="G30" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D31" t="s">
-        <v>93</v>
-      </c>
-      <c r="E31" t="s">
-        <v>95</v>
-      </c>
-      <c r="F31" t="s">
-        <v>96</v>
-      </c>
-      <c r="G31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D32" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E33" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F33" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
-        <v>114</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>118</v>
+        <v>99</v>
+      </c>
+      <c r="E34" t="s">
+        <v>100</v>
+      </c>
+      <c r="F34" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" t="s">
-        <v>100</v>
-      </c>
       <c r="D35" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>115</v>
@@ -1243,29 +1264,46 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" t="s">
+        <v>111</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>27</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>32</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>